<commit_message>
adding test types with new testcases
</commit_message>
<xml_diff>
--- a/gobusTRM.xlsx
+++ b/gobusTRM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
   <si>
     <t>REQUIREMENT TRACEABILITY MATRIX</t>
   </si>
@@ -324,12 +324,21 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>T50</t>
+  </si>
+  <si>
+    <t>T51</t>
+  </si>
+  <si>
+    <t>T52</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +385,12 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -433,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -457,6 +472,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -768,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1387,6 +1405,48 @@
         <v>93</v>
       </c>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>41</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>42</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>43</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>